<commit_message>
Update BMI PGS Calculation before sending to Nur.
</commit_message>
<xml_diff>
--- a/PGS.matching.summary_WCHS_BrCa_BMI_PGS.xlsx
+++ b/PGS.matching.summary_WCHS_BrCa_BMI_PGS.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Trait</t>
   </si>
   <si>
     <t xml:space="preserve">N.of.Variants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N.of.non_zero_Variants</t>
   </si>
   <si>
     <t xml:space="preserve">N.of.Ambg</t>
@@ -384,12 +387,13 @@
   <cols>
     <col min="1" max="1" width="9.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="13.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="9.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="13.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="15.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="22.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="9.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="13.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="15.71" hidden="0" customWidth="1"/>
-    <col min="8" max="8" width="17.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="15.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="17.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -417,135 +421,153 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
         <v>87</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>79.31</v>
+        <v>78</v>
       </c>
       <c r="G2" t="n">
-        <v>54</v>
+        <v>89.66</v>
       </c>
       <c r="H2" t="n">
-        <v>62.07</v>
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
         <v>752209</v>
       </c>
       <c r="C3" t="n">
+        <v>225012</v>
+      </c>
+      <c r="D3" t="n">
         <v>334</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.04</v>
       </c>
-      <c r="E3" t="n">
-        <v>215312</v>
-      </c>
       <c r="F3" t="n">
-        <v>28.62</v>
+        <v>215351</v>
       </c>
       <c r="G3" t="n">
-        <v>587943</v>
+        <v>95.71</v>
       </c>
       <c r="H3" t="n">
-        <v>78.16</v>
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="n">
         <v>817189</v>
       </c>
       <c r="C4" t="n">
+        <v>817189</v>
+      </c>
+      <c r="D4" t="n">
         <v>67</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.01</v>
       </c>
-      <c r="E4" t="n">
-        <v>771810</v>
-      </c>
       <c r="F4" t="n">
-        <v>94.45</v>
+        <v>771884</v>
       </c>
       <c r="G4" t="n">
-        <v>137478</v>
+        <v>94.46</v>
       </c>
       <c r="H4" t="n">
-        <v>16.82</v>
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="n">
         <v>300864</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>300864</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>292677</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>97.28</v>
+        <v>293162</v>
       </c>
       <c r="G5" t="n">
-        <v>205428</v>
+        <v>97.44</v>
       </c>
       <c r="H5" t="n">
-        <v>68.28</v>
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="n">
         <v>741723</v>
       </c>
       <c r="C6" t="n">
+        <v>382148</v>
+      </c>
+      <c r="D6" t="n">
         <v>79</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>0.01</v>
       </c>
-      <c r="E6" t="n">
-        <v>361254</v>
-      </c>
       <c r="F6" t="n">
-        <v>48.7</v>
+        <v>361296</v>
       </c>
       <c r="G6" t="n">
-        <v>579702</v>
+        <v>94.54</v>
       </c>
       <c r="H6" t="n">
-        <v>78.16</v>
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>